<commit_message>
new list of momentum stocks. backtest analyse script wip
</commit_message>
<xml_diff>
--- a/QuantStock/data/output/momentum_monthly_output.xlsx
+++ b/QuantStock/data/output/momentum_monthly_output.xlsx
@@ -61,6 +61,33 @@
     <sheet name="2020-08-28" sheetId="53" state="visible" r:id="rId53"/>
     <sheet name="2020-09-04" sheetId="54" state="visible" r:id="rId54"/>
     <sheet name="2020-09-11" sheetId="55" state="visible" r:id="rId55"/>
+    <sheet name="2020-03-201" sheetId="56" state="visible" r:id="rId56"/>
+    <sheet name="2020-03-271" sheetId="57" state="visible" r:id="rId57"/>
+    <sheet name="2020-04-031" sheetId="58" state="visible" r:id="rId58"/>
+    <sheet name="2020-04-101" sheetId="59" state="visible" r:id="rId59"/>
+    <sheet name="2020-04-171" sheetId="60" state="visible" r:id="rId60"/>
+    <sheet name="2020-04-241" sheetId="61" state="visible" r:id="rId61"/>
+    <sheet name="2020-05-011" sheetId="62" state="visible" r:id="rId62"/>
+    <sheet name="2020-05-081" sheetId="63" state="visible" r:id="rId63"/>
+    <sheet name="2020-05-151" sheetId="64" state="visible" r:id="rId64"/>
+    <sheet name="2020-05-221" sheetId="65" state="visible" r:id="rId65"/>
+    <sheet name="2020-05-291" sheetId="66" state="visible" r:id="rId66"/>
+    <sheet name="2020-06-051" sheetId="67" state="visible" r:id="rId67"/>
+    <sheet name="2020-06-121" sheetId="68" state="visible" r:id="rId68"/>
+    <sheet name="2020-06-191" sheetId="69" state="visible" r:id="rId69"/>
+    <sheet name="2020-06-261" sheetId="70" state="visible" r:id="rId70"/>
+    <sheet name="2020-07-031" sheetId="71" state="visible" r:id="rId71"/>
+    <sheet name="2020-07-101" sheetId="72" state="visible" r:id="rId72"/>
+    <sheet name="2020-07-171" sheetId="73" state="visible" r:id="rId73"/>
+    <sheet name="2020-07-241" sheetId="74" state="visible" r:id="rId74"/>
+    <sheet name="2020-07-311" sheetId="75" state="visible" r:id="rId75"/>
+    <sheet name="2020-08-071" sheetId="76" state="visible" r:id="rId76"/>
+    <sheet name="2020-08-141" sheetId="77" state="visible" r:id="rId77"/>
+    <sheet name="2020-08-211" sheetId="78" state="visible" r:id="rId78"/>
+    <sheet name="2020-08-281" sheetId="79" state="visible" r:id="rId79"/>
+    <sheet name="2020-09-041" sheetId="80" state="visible" r:id="rId80"/>
+    <sheet name="2020-09-111" sheetId="81" state="visible" r:id="rId81"/>
+    <sheet name="2020-09-18" sheetId="82" state="visible" r:id="rId82"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="0" fullCalcOnLoad="1"/>
@@ -49001,10 +49028,6 @@
           <t>ASIANPAINT.NS</t>
         </is>
       </c>
-      <c r="B43" t="inlineStr"/>
-      <c r="C43" t="inlineStr"/>
-      <c r="D43" t="inlineStr"/>
-      <c r="E43" t="inlineStr"/>
     </row>
     <row r="44">
       <c r="A44" s="2" t="inlineStr">
@@ -49012,10 +49035,6 @@
           <t>AXISBANK.NS</t>
         </is>
       </c>
-      <c r="B44" t="inlineStr"/>
-      <c r="C44" t="inlineStr"/>
-      <c r="D44" t="inlineStr"/>
-      <c r="E44" t="inlineStr"/>
     </row>
     <row r="45">
       <c r="A45" s="2" t="inlineStr">
@@ -49023,10 +49042,6 @@
           <t>COALINDIA.NS</t>
         </is>
       </c>
-      <c r="B45" t="inlineStr"/>
-      <c r="C45" t="inlineStr"/>
-      <c r="D45" t="inlineStr"/>
-      <c r="E45" t="inlineStr"/>
     </row>
     <row r="46">
       <c r="A46" s="2" t="inlineStr">
@@ -49034,10 +49049,6 @@
           <t>KOTAKBANK.NS</t>
         </is>
       </c>
-      <c r="B46" t="inlineStr"/>
-      <c r="C46" t="inlineStr"/>
-      <c r="D46" t="inlineStr"/>
-      <c r="E46" t="inlineStr"/>
     </row>
     <row r="47">
       <c r="A47" s="2" t="inlineStr">
@@ -49045,10 +49056,6 @@
           <t>RELIANCE.NS</t>
         </is>
       </c>
-      <c r="B47" t="inlineStr"/>
-      <c r="C47" t="inlineStr"/>
-      <c r="D47" t="inlineStr"/>
-      <c r="E47" t="inlineStr"/>
     </row>
     <row r="48">
       <c r="A48" s="2" t="inlineStr">
@@ -49056,10 +49063,6 @@
           <t>TATASTEEL.NS</t>
         </is>
       </c>
-      <c r="B48" t="inlineStr"/>
-      <c r="C48" t="inlineStr"/>
-      <c r="D48" t="inlineStr"/>
-      <c r="E48" t="inlineStr"/>
     </row>
     <row r="49">
       <c r="A49" s="2" t="inlineStr">
@@ -49067,10 +49070,6 @@
           <t>TECHM.NS</t>
         </is>
       </c>
-      <c r="B49" t="inlineStr"/>
-      <c r="C49" t="inlineStr"/>
-      <c r="D49" t="inlineStr"/>
-      <c r="E49" t="inlineStr"/>
     </row>
     <row r="50">
       <c r="A50" s="2" t="inlineStr">
@@ -49078,10 +49077,6 @@
           <t>TITAN.NS</t>
         </is>
       </c>
-      <c r="B50" t="inlineStr"/>
-      <c r="C50" t="inlineStr"/>
-      <c r="D50" t="inlineStr"/>
-      <c r="E50" t="inlineStr"/>
     </row>
     <row r="51">
       <c r="A51" s="2" t="inlineStr">
@@ -49089,10 +49084,418 @@
           <t>WIPRO.NS</t>
         </is>
       </c>
-      <c r="B51" t="inlineStr"/>
-      <c r="C51" t="inlineStr"/>
-      <c r="D51" t="inlineStr"/>
-      <c r="E51" t="inlineStr"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet56.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:E4"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="2" t="inlineStr">
+        <is>
+          <t>MOMENTUM_ATH</t>
+        </is>
+      </c>
+      <c r="B1" s="2" t="inlineStr">
+        <is>
+          <t>2020-02-20</t>
+        </is>
+      </c>
+      <c r="C1" s="2" t="inlineStr">
+        <is>
+          <t>2020-03-20</t>
+        </is>
+      </c>
+      <c r="D1" s="2" t="inlineStr">
+        <is>
+          <t>Change</t>
+        </is>
+      </c>
+      <c r="E1" s="2" t="inlineStr">
+        <is>
+          <t>% Change</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" s="2" t="inlineStr">
+        <is>
+          <t>ASIANPAINT.NS</t>
+        </is>
+      </c>
+      <c r="B2" t="n">
+        <v>1830.46</v>
+      </c>
+      <c r="C2" t="n">
+        <v>1738.75</v>
+      </c>
+      <c r="D2" t="n">
+        <v>-91.70999999999999</v>
+      </c>
+      <c r="E2" t="n">
+        <v>-5.01</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" s="2" t="inlineStr">
+        <is>
+          <t>ADANIPORTS.NS</t>
+        </is>
+      </c>
+      <c r="B3" t="n">
+        <v>366.8</v>
+      </c>
+      <c r="C3" t="n">
+        <v>256.4</v>
+      </c>
+      <c r="D3" t="n">
+        <v>-110.4</v>
+      </c>
+      <c r="E3" t="n">
+        <v>-30.1</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" s="2" t="inlineStr">
+        <is>
+          <t>AXISBANK.NS</t>
+        </is>
+      </c>
+      <c r="B4" t="n">
+        <v>744.3</v>
+      </c>
+      <c r="C4" t="n">
+        <v>428.15</v>
+      </c>
+      <c r="D4" t="n">
+        <v>-316.15</v>
+      </c>
+      <c r="E4" t="n">
+        <v>-42.48</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet57.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:E4"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="2" t="inlineStr">
+        <is>
+          <t>MOMENTUM_ATH</t>
+        </is>
+      </c>
+      <c r="B1" s="2" t="inlineStr">
+        <is>
+          <t>2020-02-27</t>
+        </is>
+      </c>
+      <c r="C1" s="2" t="inlineStr">
+        <is>
+          <t>2020-03-27</t>
+        </is>
+      </c>
+      <c r="D1" s="2" t="inlineStr">
+        <is>
+          <t>Change</t>
+        </is>
+      </c>
+      <c r="E1" s="2" t="inlineStr">
+        <is>
+          <t>% Change</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" s="2" t="inlineStr">
+        <is>
+          <t>ASIANPAINT.NS</t>
+        </is>
+      </c>
+      <c r="B2" t="n">
+        <v>1832</v>
+      </c>
+      <c r="C2" t="n">
+        <v>1600.29</v>
+      </c>
+      <c r="D2" t="n">
+        <v>-231.71</v>
+      </c>
+      <c r="E2" t="n">
+        <v>-12.65</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" s="2" t="inlineStr">
+        <is>
+          <t>ADANIPORTS.NS</t>
+        </is>
+      </c>
+      <c r="B3" t="n">
+        <v>349.83</v>
+      </c>
+      <c r="C3" t="n">
+        <v>251.3</v>
+      </c>
+      <c r="D3" t="n">
+        <v>-98.53</v>
+      </c>
+      <c r="E3" t="n">
+        <v>-28.17</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" s="2" t="inlineStr">
+        <is>
+          <t>AXISBANK.NS</t>
+        </is>
+      </c>
+      <c r="B4" t="n">
+        <v>735.85</v>
+      </c>
+      <c r="C4" t="n">
+        <v>359.75</v>
+      </c>
+      <c r="D4" t="n">
+        <v>-376.1</v>
+      </c>
+      <c r="E4" t="n">
+        <v>-51.11</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet58.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:E4"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="2" t="inlineStr">
+        <is>
+          <t>MOMENTUM_ATH</t>
+        </is>
+      </c>
+      <c r="B1" s="2" t="inlineStr">
+        <is>
+          <t>2020-03-03</t>
+        </is>
+      </c>
+      <c r="C1" s="2" t="inlineStr">
+        <is>
+          <t>2020-04-03</t>
+        </is>
+      </c>
+      <c r="D1" s="2" t="inlineStr">
+        <is>
+          <t>Change</t>
+        </is>
+      </c>
+      <c r="E1" s="2" t="inlineStr">
+        <is>
+          <t>% Change</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" s="2" t="inlineStr">
+        <is>
+          <t>ASIANPAINT.NS</t>
+        </is>
+      </c>
+      <c r="B2" t="n">
+        <v>1796.22</v>
+      </c>
+      <c r="C2" t="n">
+        <v>1517.24</v>
+      </c>
+      <c r="D2" t="n">
+        <v>-278.98</v>
+      </c>
+      <c r="E2" t="n">
+        <v>-15.53</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" s="2" t="inlineStr">
+        <is>
+          <t>ADANIPORTS.NS</t>
+        </is>
+      </c>
+      <c r="B3" t="n">
+        <v>343.5</v>
+      </c>
+      <c r="C3" t="n">
+        <v>244.8</v>
+      </c>
+      <c r="D3" t="n">
+        <v>-98.7</v>
+      </c>
+      <c r="E3" t="n">
+        <v>-28.73</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" s="2" t="inlineStr">
+        <is>
+          <t>AXISBANK.NS</t>
+        </is>
+      </c>
+      <c r="B4" t="n">
+        <v>687.15</v>
+      </c>
+      <c r="C4" t="n">
+        <v>325.45</v>
+      </c>
+      <c r="D4" t="n">
+        <v>-361.7</v>
+      </c>
+      <c r="E4" t="n">
+        <v>-52.64</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet59.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:E4"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="2" t="inlineStr">
+        <is>
+          <t>MOMENTUM_ATH</t>
+        </is>
+      </c>
+      <c r="B1" s="2" t="inlineStr">
+        <is>
+          <t>2020-03-11</t>
+        </is>
+      </c>
+      <c r="C1" s="2" t="inlineStr">
+        <is>
+          <t>2020-04-13</t>
+        </is>
+      </c>
+      <c r="D1" s="2" t="inlineStr">
+        <is>
+          <t>Change</t>
+        </is>
+      </c>
+      <c r="E1" s="2" t="inlineStr">
+        <is>
+          <t>% Change</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" s="2" t="inlineStr">
+        <is>
+          <t>ASIANPAINT.NS</t>
+        </is>
+      </c>
+      <c r="B2" t="n">
+        <v>1878.32</v>
+      </c>
+      <c r="C2" t="n">
+        <v>1676.8</v>
+      </c>
+      <c r="D2" t="n">
+        <v>-201.51</v>
+      </c>
+      <c r="E2" t="n">
+        <v>-10.73</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" s="2" t="inlineStr">
+        <is>
+          <t>ADANIPORTS.NS</t>
+        </is>
+      </c>
+      <c r="B3" t="n">
+        <v>316.7</v>
+      </c>
+      <c r="C3" t="n">
+        <v>262.85</v>
+      </c>
+      <c r="D3" t="n">
+        <v>-53.85</v>
+      </c>
+      <c r="E3" t="n">
+        <v>-17</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" s="2" t="inlineStr">
+        <is>
+          <t>AXISBANK.NS</t>
+        </is>
+      </c>
+      <c r="B4" t="n">
+        <v>619.35</v>
+      </c>
+      <c r="C4" t="n">
+        <v>418.95</v>
+      </c>
+      <c r="D4" t="n">
+        <v>-200.4</v>
+      </c>
+      <c r="E4" t="n">
+        <v>-32.36</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -50095,6 +50498,1036 @@
 </worksheet>
 </file>
 
+<file path=xl/worksheets/sheet60.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:E4"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="2" t="inlineStr">
+        <is>
+          <t>MOMENTUM_ATH</t>
+        </is>
+      </c>
+      <c r="B1" s="2" t="inlineStr">
+        <is>
+          <t>2020-03-17</t>
+        </is>
+      </c>
+      <c r="C1" s="2" t="inlineStr">
+        <is>
+          <t>2020-04-17</t>
+        </is>
+      </c>
+      <c r="D1" s="2" t="inlineStr">
+        <is>
+          <t>Change</t>
+        </is>
+      </c>
+      <c r="E1" s="2" t="inlineStr">
+        <is>
+          <t>% Change</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" s="2" t="inlineStr">
+        <is>
+          <t>ASIANPAINT.NS</t>
+        </is>
+      </c>
+      <c r="B2" t="n">
+        <v>1727.43</v>
+      </c>
+      <c r="C2" t="n">
+        <v>1752.02</v>
+      </c>
+      <c r="D2" t="n">
+        <v>24.59</v>
+      </c>
+      <c r="E2" t="n">
+        <v>1.42</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" s="2" t="inlineStr">
+        <is>
+          <t>ADANIPORTS.NS</t>
+        </is>
+      </c>
+      <c r="B3" t="n">
+        <v>267.15</v>
+      </c>
+      <c r="C3" t="n">
+        <v>268.15</v>
+      </c>
+      <c r="D3" t="n">
+        <v>1</v>
+      </c>
+      <c r="E3" t="n">
+        <v>0.37</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" s="2" t="inlineStr">
+        <is>
+          <t>AXISBANK.NS</t>
+        </is>
+      </c>
+      <c r="B4" t="n">
+        <v>488.35</v>
+      </c>
+      <c r="C4" t="n">
+        <v>478.8</v>
+      </c>
+      <c r="D4" t="n">
+        <v>-9.550000000000001</v>
+      </c>
+      <c r="E4" t="n">
+        <v>-1.96</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet61.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:E4"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="2" t="inlineStr">
+        <is>
+          <t>MOMENTUM_ATH</t>
+        </is>
+      </c>
+      <c r="B1" s="2" t="inlineStr">
+        <is>
+          <t>2020-03-24</t>
+        </is>
+      </c>
+      <c r="C1" s="2" t="inlineStr">
+        <is>
+          <t>2020-04-24</t>
+        </is>
+      </c>
+      <c r="D1" s="2" t="inlineStr">
+        <is>
+          <t>Change</t>
+        </is>
+      </c>
+      <c r="E1" s="2" t="inlineStr">
+        <is>
+          <t>% Change</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" s="2" t="inlineStr">
+        <is>
+          <t>AXISBANK.NS</t>
+        </is>
+      </c>
+      <c r="B2" t="n">
+        <v>303.15</v>
+      </c>
+      <c r="C2" t="n">
+        <v>403.95</v>
+      </c>
+      <c r="D2" t="n">
+        <v>100.8</v>
+      </c>
+      <c r="E2" t="n">
+        <v>33.25</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" s="2" t="inlineStr">
+        <is>
+          <t>ASIANPAINT.NS</t>
+        </is>
+      </c>
+      <c r="B3" t="n">
+        <v>1521.18</v>
+      </c>
+      <c r="C3" t="n">
+        <v>1823.15</v>
+      </c>
+      <c r="D3" t="n">
+        <v>301.97</v>
+      </c>
+      <c r="E3" t="n">
+        <v>19.85</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" s="2" t="inlineStr">
+        <is>
+          <t>ADANIPORTS.NS</t>
+        </is>
+      </c>
+      <c r="B4" t="n">
+        <v>231.75</v>
+      </c>
+      <c r="C4" t="n">
+        <v>270.65</v>
+      </c>
+      <c r="D4" t="n">
+        <v>38.9</v>
+      </c>
+      <c r="E4" t="n">
+        <v>16.79</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet62.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:E4"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="2" t="inlineStr">
+        <is>
+          <t>MOMENTUM_ATH</t>
+        </is>
+      </c>
+      <c r="B1" s="2" t="inlineStr">
+        <is>
+          <t>2020-04-01</t>
+        </is>
+      </c>
+      <c r="C1" s="2" t="inlineStr">
+        <is>
+          <t>2020-05-04</t>
+        </is>
+      </c>
+      <c r="D1" s="2" t="inlineStr">
+        <is>
+          <t>Change</t>
+        </is>
+      </c>
+      <c r="E1" s="2" t="inlineStr">
+        <is>
+          <t>% Change</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" s="2" t="inlineStr">
+        <is>
+          <t>AXISBANK.NS</t>
+        </is>
+      </c>
+      <c r="B2" t="n">
+        <v>358.65</v>
+      </c>
+      <c r="C2" t="n">
+        <v>402.8</v>
+      </c>
+      <c r="D2" t="n">
+        <v>44.15</v>
+      </c>
+      <c r="E2" t="n">
+        <v>12.31</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" s="2" t="inlineStr">
+        <is>
+          <t>ADANIPORTS.NS</t>
+        </is>
+      </c>
+      <c r="B3" t="n">
+        <v>244.8</v>
+      </c>
+      <c r="C3" t="n">
+        <v>266.35</v>
+      </c>
+      <c r="D3" t="n">
+        <v>21.55</v>
+      </c>
+      <c r="E3" t="n">
+        <v>8.800000000000001</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" s="2" t="inlineStr">
+        <is>
+          <t>ASIANPAINT.NS</t>
+        </is>
+      </c>
+      <c r="B4" t="n">
+        <v>1599.34</v>
+      </c>
+      <c r="C4" t="n">
+        <v>1672.76</v>
+      </c>
+      <c r="D4" t="n">
+        <v>73.42</v>
+      </c>
+      <c r="E4" t="n">
+        <v>4.59</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet63.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:E4"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="2" t="inlineStr">
+        <is>
+          <t>MOMENTUM_ATH</t>
+        </is>
+      </c>
+      <c r="B1" s="2" t="inlineStr">
+        <is>
+          <t>2020-04-08</t>
+        </is>
+      </c>
+      <c r="C1" s="2" t="inlineStr">
+        <is>
+          <t>2020-05-08</t>
+        </is>
+      </c>
+      <c r="D1" s="2" t="inlineStr">
+        <is>
+          <t>Change</t>
+        </is>
+      </c>
+      <c r="E1" s="2" t="inlineStr">
+        <is>
+          <t>% Change</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" s="2" t="inlineStr">
+        <is>
+          <t>ADANIPORTS.NS</t>
+        </is>
+      </c>
+      <c r="B2" t="n">
+        <v>250.85</v>
+      </c>
+      <c r="C2" t="n">
+        <v>285.05</v>
+      </c>
+      <c r="D2" t="n">
+        <v>34.2</v>
+      </c>
+      <c r="E2" t="n">
+        <v>13.63</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" s="2" t="inlineStr">
+        <is>
+          <t>ASIANPAINT.NS</t>
+        </is>
+      </c>
+      <c r="B3" t="n">
+        <v>1605.08</v>
+      </c>
+      <c r="C3" t="n">
+        <v>1574.6</v>
+      </c>
+      <c r="D3" t="n">
+        <v>-30.48</v>
+      </c>
+      <c r="E3" t="n">
+        <v>-1.9</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" s="2" t="inlineStr">
+        <is>
+          <t>AXISBANK.NS</t>
+        </is>
+      </c>
+      <c r="B4" t="n">
+        <v>391.35</v>
+      </c>
+      <c r="C4" t="n">
+        <v>382.05</v>
+      </c>
+      <c r="D4" t="n">
+        <v>-9.300000000000001</v>
+      </c>
+      <c r="E4" t="n">
+        <v>-2.38</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet64.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:E4"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="2" t="inlineStr">
+        <is>
+          <t>MOMENTUM_ATH</t>
+        </is>
+      </c>
+      <c r="B1" s="2" t="inlineStr">
+        <is>
+          <t>2020-04-15</t>
+        </is>
+      </c>
+      <c r="C1" s="2" t="inlineStr">
+        <is>
+          <t>2020-05-15</t>
+        </is>
+      </c>
+      <c r="D1" s="2" t="inlineStr">
+        <is>
+          <t>Change</t>
+        </is>
+      </c>
+      <c r="E1" s="2" t="inlineStr">
+        <is>
+          <t>% Change</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" s="2" t="inlineStr">
+        <is>
+          <t>ADANIPORTS.NS</t>
+        </is>
+      </c>
+      <c r="B2" t="n">
+        <v>268.9</v>
+      </c>
+      <c r="C2" t="n">
+        <v>309.25</v>
+      </c>
+      <c r="D2" t="n">
+        <v>40.35</v>
+      </c>
+      <c r="E2" t="n">
+        <v>15.01</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" s="2" t="inlineStr">
+        <is>
+          <t>AXISBANK.NS</t>
+        </is>
+      </c>
+      <c r="B3" t="n">
+        <v>417.3</v>
+      </c>
+      <c r="C3" t="n">
+        <v>388.55</v>
+      </c>
+      <c r="D3" t="n">
+        <v>-28.75</v>
+      </c>
+      <c r="E3" t="n">
+        <v>-6.89</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" s="2" t="inlineStr">
+        <is>
+          <t>ASIANPAINT.NS</t>
+        </is>
+      </c>
+      <c r="B4" t="n">
+        <v>1714.06</v>
+      </c>
+      <c r="C4" t="n">
+        <v>1549.21</v>
+      </c>
+      <c r="D4" t="n">
+        <v>-164.85</v>
+      </c>
+      <c r="E4" t="n">
+        <v>-9.619999999999999</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet65.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:E4"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="2" t="inlineStr">
+        <is>
+          <t>MOMENTUM_ATH</t>
+        </is>
+      </c>
+      <c r="B1" s="2" t="inlineStr">
+        <is>
+          <t>2020-04-22</t>
+        </is>
+      </c>
+      <c r="C1" s="2" t="inlineStr">
+        <is>
+          <t>2020-05-22</t>
+        </is>
+      </c>
+      <c r="D1" s="2" t="inlineStr">
+        <is>
+          <t>Change</t>
+        </is>
+      </c>
+      <c r="E1" s="2" t="inlineStr">
+        <is>
+          <t>% Change</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" s="2" t="inlineStr">
+        <is>
+          <t>ADANIPORTS.NS</t>
+        </is>
+      </c>
+      <c r="B2" t="n">
+        <v>271.9</v>
+      </c>
+      <c r="C2" t="n">
+        <v>310.6</v>
+      </c>
+      <c r="D2" t="n">
+        <v>38.7</v>
+      </c>
+      <c r="E2" t="n">
+        <v>14.23</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" s="2" t="inlineStr">
+        <is>
+          <t>ASIANPAINT.NS</t>
+        </is>
+      </c>
+      <c r="B3" t="n">
+        <v>1808.64</v>
+      </c>
+      <c r="C3" t="n">
+        <v>1614.01</v>
+      </c>
+      <c r="D3" t="n">
+        <v>-194.63</v>
+      </c>
+      <c r="E3" t="n">
+        <v>-10.76</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" s="2" t="inlineStr">
+        <is>
+          <t>AXISBANK.NS</t>
+        </is>
+      </c>
+      <c r="B4" t="n">
+        <v>431.15</v>
+      </c>
+      <c r="C4" t="n">
+        <v>336.95</v>
+      </c>
+      <c r="D4" t="n">
+        <v>-94.2</v>
+      </c>
+      <c r="E4" t="n">
+        <v>-21.85</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet66.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:E4"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="2" t="inlineStr">
+        <is>
+          <t>MOMENTUM_ATH</t>
+        </is>
+      </c>
+      <c r="B1" s="2" t="inlineStr">
+        <is>
+          <t>2020-04-29</t>
+        </is>
+      </c>
+      <c r="C1" s="2" t="inlineStr">
+        <is>
+          <t>2020-05-29</t>
+        </is>
+      </c>
+      <c r="D1" s="2" t="inlineStr">
+        <is>
+          <t>Change</t>
+        </is>
+      </c>
+      <c r="E1" s="2" t="inlineStr">
+        <is>
+          <t>% Change</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" s="2" t="inlineStr">
+        <is>
+          <t>ADANIPORTS.NS</t>
+        </is>
+      </c>
+      <c r="B2" t="n">
+        <v>287.65</v>
+      </c>
+      <c r="C2" t="n">
+        <v>323.8</v>
+      </c>
+      <c r="D2" t="n">
+        <v>36.15</v>
+      </c>
+      <c r="E2" t="n">
+        <v>12.57</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" s="2" t="inlineStr">
+        <is>
+          <t>ASIANPAINT.NS</t>
+        </is>
+      </c>
+      <c r="B3" t="n">
+        <v>1763.24</v>
+      </c>
+      <c r="C3" t="n">
+        <v>1679.05</v>
+      </c>
+      <c r="D3" t="n">
+        <v>-84.2</v>
+      </c>
+      <c r="E3" t="n">
+        <v>-4.78</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" s="2" t="inlineStr">
+        <is>
+          <t>AXISBANK.NS</t>
+        </is>
+      </c>
+      <c r="B4" t="n">
+        <v>439.1</v>
+      </c>
+      <c r="C4" t="n">
+        <v>384.95</v>
+      </c>
+      <c r="D4" t="n">
+        <v>-54.15</v>
+      </c>
+      <c r="E4" t="n">
+        <v>-12.33</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet67.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:E4"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="2" t="inlineStr">
+        <is>
+          <t>MOMENTUM_ATH</t>
+        </is>
+      </c>
+      <c r="B1" s="2" t="inlineStr">
+        <is>
+          <t>2020-05-05</t>
+        </is>
+      </c>
+      <c r="C1" s="2" t="inlineStr">
+        <is>
+          <t>2020-06-05</t>
+        </is>
+      </c>
+      <c r="D1" s="2" t="inlineStr">
+        <is>
+          <t>Change</t>
+        </is>
+      </c>
+      <c r="E1" s="2" t="inlineStr">
+        <is>
+          <t>% Change</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" s="2" t="inlineStr">
+        <is>
+          <t>ADANIPORTS.NS</t>
+        </is>
+      </c>
+      <c r="B2" t="n">
+        <v>263.1</v>
+      </c>
+      <c r="C2" t="n">
+        <v>341.15</v>
+      </c>
+      <c r="D2" t="n">
+        <v>78.05</v>
+      </c>
+      <c r="E2" t="n">
+        <v>29.67</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" s="2" t="inlineStr">
+        <is>
+          <t>AXISBANK.NS</t>
+        </is>
+      </c>
+      <c r="B3" t="n">
+        <v>389</v>
+      </c>
+      <c r="C3" t="n">
+        <v>405.3</v>
+      </c>
+      <c r="D3" t="n">
+        <v>16.3</v>
+      </c>
+      <c r="E3" t="n">
+        <v>4.19</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" s="2" t="inlineStr">
+        <is>
+          <t>ASIANPAINT.NS</t>
+        </is>
+      </c>
+      <c r="B4" t="n">
+        <v>1615.25</v>
+      </c>
+      <c r="C4" t="n">
+        <v>1634.61</v>
+      </c>
+      <c r="D4" t="n">
+        <v>19.35</v>
+      </c>
+      <c r="E4" t="n">
+        <v>1.2</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet68.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:E4"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="2" t="inlineStr">
+        <is>
+          <t>MOMENTUM_ATH</t>
+        </is>
+      </c>
+      <c r="B1" s="2" t="inlineStr">
+        <is>
+          <t>2020-05-12</t>
+        </is>
+      </c>
+      <c r="C1" s="2" t="inlineStr">
+        <is>
+          <t>2020-06-12</t>
+        </is>
+      </c>
+      <c r="D1" s="2" t="inlineStr">
+        <is>
+          <t>Change</t>
+        </is>
+      </c>
+      <c r="E1" s="2" t="inlineStr">
+        <is>
+          <t>% Change</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" s="2" t="inlineStr">
+        <is>
+          <t>ADANIPORTS.NS</t>
+        </is>
+      </c>
+      <c r="B2" t="n">
+        <v>291.5</v>
+      </c>
+      <c r="C2" t="n">
+        <v>345.3</v>
+      </c>
+      <c r="D2" t="n">
+        <v>53.8</v>
+      </c>
+      <c r="E2" t="n">
+        <v>18.46</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" s="2" t="inlineStr">
+        <is>
+          <t>ASIANPAINT.NS</t>
+        </is>
+      </c>
+      <c r="B3" t="n">
+        <v>1519.68</v>
+      </c>
+      <c r="C3" t="n">
+        <v>1633.41</v>
+      </c>
+      <c r="D3" t="n">
+        <v>113.73</v>
+      </c>
+      <c r="E3" t="n">
+        <v>7.48</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" s="2" t="inlineStr">
+        <is>
+          <t>AXISBANK.NS</t>
+        </is>
+      </c>
+      <c r="B4" t="n">
+        <v>386.85</v>
+      </c>
+      <c r="C4" t="n">
+        <v>408</v>
+      </c>
+      <c r="D4" t="n">
+        <v>21.15</v>
+      </c>
+      <c r="E4" t="n">
+        <v>5.47</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet69.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:E4"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="2" t="inlineStr">
+        <is>
+          <t>MOMENTUM_ATH</t>
+        </is>
+      </c>
+      <c r="B1" s="2" t="inlineStr">
+        <is>
+          <t>2020-05-19</t>
+        </is>
+      </c>
+      <c r="C1" s="2" t="inlineStr">
+        <is>
+          <t>2020-06-19</t>
+        </is>
+      </c>
+      <c r="D1" s="2" t="inlineStr">
+        <is>
+          <t>Change</t>
+        </is>
+      </c>
+      <c r="E1" s="2" t="inlineStr">
+        <is>
+          <t>% Change</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" s="2" t="inlineStr">
+        <is>
+          <t>AXISBANK.NS</t>
+        </is>
+      </c>
+      <c r="B2" t="n">
+        <v>354.5</v>
+      </c>
+      <c r="C2" t="n">
+        <v>417.05</v>
+      </c>
+      <c r="D2" t="n">
+        <v>62.55</v>
+      </c>
+      <c r="E2" t="n">
+        <v>17.64</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" s="2" t="inlineStr">
+        <is>
+          <t>ADANIPORTS.NS</t>
+        </is>
+      </c>
+      <c r="B3" t="n">
+        <v>319.2</v>
+      </c>
+      <c r="C3" t="n">
+        <v>348.9</v>
+      </c>
+      <c r="D3" t="n">
+        <v>29.7</v>
+      </c>
+      <c r="E3" t="n">
+        <v>9.300000000000001</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" s="2" t="inlineStr">
+        <is>
+          <t>ASIANPAINT.NS</t>
+        </is>
+      </c>
+      <c r="B4" t="n">
+        <v>1500.33</v>
+      </c>
+      <c r="C4" t="n">
+        <v>1618.59</v>
+      </c>
+      <c r="D4" t="n">
+        <v>118.26</v>
+      </c>
+      <c r="E4" t="n">
+        <v>7.88</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
@@ -51084,6 +52517,1036 @@
       </c>
       <c r="E51" t="n">
         <v>-31.58</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet70.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:E4"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="2" t="inlineStr">
+        <is>
+          <t>MOMENTUM_ATH</t>
+        </is>
+      </c>
+      <c r="B1" s="2" t="inlineStr">
+        <is>
+          <t>2020-05-26</t>
+        </is>
+      </c>
+      <c r="C1" s="2" t="inlineStr">
+        <is>
+          <t>2020-06-26</t>
+        </is>
+      </c>
+      <c r="D1" s="2" t="inlineStr">
+        <is>
+          <t>Change</t>
+        </is>
+      </c>
+      <c r="E1" s="2" t="inlineStr">
+        <is>
+          <t>% Change</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" s="2" t="inlineStr">
+        <is>
+          <t>AXISBANK.NS</t>
+        </is>
+      </c>
+      <c r="B2" t="n">
+        <v>341.3</v>
+      </c>
+      <c r="C2" t="n">
+        <v>424.85</v>
+      </c>
+      <c r="D2" t="n">
+        <v>83.55</v>
+      </c>
+      <c r="E2" t="n">
+        <v>24.48</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" s="2" t="inlineStr">
+        <is>
+          <t>ADANIPORTS.NS</t>
+        </is>
+      </c>
+      <c r="B3" t="n">
+        <v>315.6</v>
+      </c>
+      <c r="C3" t="n">
+        <v>343.2</v>
+      </c>
+      <c r="D3" t="n">
+        <v>27.6</v>
+      </c>
+      <c r="E3" t="n">
+        <v>8.75</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" s="2" t="inlineStr">
+        <is>
+          <t>ASIANPAINT.NS</t>
+        </is>
+      </c>
+      <c r="B4" t="n">
+        <v>1625.93</v>
+      </c>
+      <c r="C4" t="n">
+        <v>1682.69</v>
+      </c>
+      <c r="D4" t="n">
+        <v>56.76</v>
+      </c>
+      <c r="E4" t="n">
+        <v>3.49</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet71.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:E4"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="2" t="inlineStr">
+        <is>
+          <t>MOMENTUM_ATH</t>
+        </is>
+      </c>
+      <c r="B1" s="2" t="inlineStr">
+        <is>
+          <t>2020-06-03</t>
+        </is>
+      </c>
+      <c r="C1" s="2" t="inlineStr">
+        <is>
+          <t>2020-07-03</t>
+        </is>
+      </c>
+      <c r="D1" s="2" t="inlineStr">
+        <is>
+          <t>Change</t>
+        </is>
+      </c>
+      <c r="E1" s="2" t="inlineStr">
+        <is>
+          <t>% Change</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" s="2" t="inlineStr">
+        <is>
+          <t>ADANIPORTS.NS</t>
+        </is>
+      </c>
+      <c r="B2" t="n">
+        <v>339.55</v>
+      </c>
+      <c r="C2" t="n">
+        <v>360.4</v>
+      </c>
+      <c r="D2" t="n">
+        <v>20.85</v>
+      </c>
+      <c r="E2" t="n">
+        <v>6.14</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" s="2" t="inlineStr">
+        <is>
+          <t>AXISBANK.NS</t>
+        </is>
+      </c>
+      <c r="B3" t="n">
+        <v>409.55</v>
+      </c>
+      <c r="C3" t="n">
+        <v>428.45</v>
+      </c>
+      <c r="D3" t="n">
+        <v>18.9</v>
+      </c>
+      <c r="E3" t="n">
+        <v>4.61</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" s="2" t="inlineStr">
+        <is>
+          <t>ASIANPAINT.NS</t>
+        </is>
+      </c>
+      <c r="B4" t="n">
+        <v>1712.42</v>
+      </c>
+      <c r="C4" t="n">
+        <v>1691.57</v>
+      </c>
+      <c r="D4" t="n">
+        <v>-20.85</v>
+      </c>
+      <c r="E4" t="n">
+        <v>-1.22</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet72.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:E4"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="2" t="inlineStr">
+        <is>
+          <t>MOMENTUM_ATH</t>
+        </is>
+      </c>
+      <c r="B1" s="2" t="inlineStr">
+        <is>
+          <t>2020-06-10</t>
+        </is>
+      </c>
+      <c r="C1" s="2" t="inlineStr">
+        <is>
+          <t>2020-07-10</t>
+        </is>
+      </c>
+      <c r="D1" s="2" t="inlineStr">
+        <is>
+          <t>Change</t>
+        </is>
+      </c>
+      <c r="E1" s="2" t="inlineStr">
+        <is>
+          <t>% Change</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" s="2" t="inlineStr">
+        <is>
+          <t>ASIANPAINT.NS</t>
+        </is>
+      </c>
+      <c r="B2" t="n">
+        <v>1632.01</v>
+      </c>
+      <c r="C2" t="n">
+        <v>1699.4</v>
+      </c>
+      <c r="D2" t="n">
+        <v>67.39</v>
+      </c>
+      <c r="E2" t="n">
+        <v>4.13</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" s="2" t="inlineStr">
+        <is>
+          <t>AXISBANK.NS</t>
+        </is>
+      </c>
+      <c r="B3" t="n">
+        <v>427.45</v>
+      </c>
+      <c r="C3" t="n">
+        <v>439.6</v>
+      </c>
+      <c r="D3" t="n">
+        <v>12.15</v>
+      </c>
+      <c r="E3" t="n">
+        <v>2.84</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" s="2" t="inlineStr">
+        <is>
+          <t>ADANIPORTS.NS</t>
+        </is>
+      </c>
+      <c r="B4" t="n">
+        <v>346.55</v>
+      </c>
+      <c r="C4" t="n">
+        <v>334.95</v>
+      </c>
+      <c r="D4" t="n">
+        <v>-11.6</v>
+      </c>
+      <c r="E4" t="n">
+        <v>-3.35</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet73.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:E4"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="2" t="inlineStr">
+        <is>
+          <t>MOMENTUM_ATH</t>
+        </is>
+      </c>
+      <c r="B1" s="2" t="inlineStr">
+        <is>
+          <t>2020-06-17</t>
+        </is>
+      </c>
+      <c r="C1" s="2" t="inlineStr">
+        <is>
+          <t>2020-07-17</t>
+        </is>
+      </c>
+      <c r="D1" s="2" t="inlineStr">
+        <is>
+          <t>Change</t>
+        </is>
+      </c>
+      <c r="E1" s="2" t="inlineStr">
+        <is>
+          <t>% Change</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" s="2" t="inlineStr">
+        <is>
+          <t>AXISBANK.NS</t>
+        </is>
+      </c>
+      <c r="B2" t="n">
+        <v>389.6</v>
+      </c>
+      <c r="C2" t="n">
+        <v>433.1</v>
+      </c>
+      <c r="D2" t="n">
+        <v>43.5</v>
+      </c>
+      <c r="E2" t="n">
+        <v>11.17</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" s="2" t="inlineStr">
+        <is>
+          <t>ASIANPAINT.NS</t>
+        </is>
+      </c>
+      <c r="B3" t="n">
+        <v>1591.56</v>
+      </c>
+      <c r="C3" t="n">
+        <v>1713.76</v>
+      </c>
+      <c r="D3" t="n">
+        <v>122.21</v>
+      </c>
+      <c r="E3" t="n">
+        <v>7.68</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" s="2" t="inlineStr">
+        <is>
+          <t>ADANIPORTS.NS</t>
+        </is>
+      </c>
+      <c r="B4" t="n">
+        <v>341.3</v>
+      </c>
+      <c r="C4" t="n">
+        <v>313</v>
+      </c>
+      <c r="D4" t="n">
+        <v>-28.3</v>
+      </c>
+      <c r="E4" t="n">
+        <v>-8.289999999999999</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet74.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:E4"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="2" t="inlineStr">
+        <is>
+          <t>MOMENTUM_ATH</t>
+        </is>
+      </c>
+      <c r="B1" s="2" t="inlineStr">
+        <is>
+          <t>2020-06-24</t>
+        </is>
+      </c>
+      <c r="C1" s="2" t="inlineStr">
+        <is>
+          <t>2020-07-24</t>
+        </is>
+      </c>
+      <c r="D1" s="2" t="inlineStr">
+        <is>
+          <t>Change</t>
+        </is>
+      </c>
+      <c r="E1" s="2" t="inlineStr">
+        <is>
+          <t>% Change</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" s="2" t="inlineStr">
+        <is>
+          <t>AXISBANK.NS</t>
+        </is>
+      </c>
+      <c r="B2" t="n">
+        <v>424.65</v>
+      </c>
+      <c r="C2" t="n">
+        <v>445.6</v>
+      </c>
+      <c r="D2" t="n">
+        <v>20.95</v>
+      </c>
+      <c r="E2" t="n">
+        <v>4.93</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" s="2" t="inlineStr">
+        <is>
+          <t>ASIANPAINT.NS</t>
+        </is>
+      </c>
+      <c r="B3" t="n">
+        <v>1743.04</v>
+      </c>
+      <c r="C3" t="n">
+        <v>1709.44</v>
+      </c>
+      <c r="D3" t="n">
+        <v>-33.6</v>
+      </c>
+      <c r="E3" t="n">
+        <v>-1.93</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" s="2" t="inlineStr">
+        <is>
+          <t>ADANIPORTS.NS</t>
+        </is>
+      </c>
+      <c r="B4" t="n">
+        <v>351.85</v>
+      </c>
+      <c r="C4" t="n">
+        <v>309.4</v>
+      </c>
+      <c r="D4" t="n">
+        <v>-42.45</v>
+      </c>
+      <c r="E4" t="n">
+        <v>-12.06</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet75.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:E4"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="2" t="inlineStr">
+        <is>
+          <t>MOMENTUM_ATH</t>
+        </is>
+      </c>
+      <c r="B1" s="2" t="inlineStr">
+        <is>
+          <t>2020-06-30</t>
+        </is>
+      </c>
+      <c r="C1" s="2" t="inlineStr">
+        <is>
+          <t>2020-07-31</t>
+        </is>
+      </c>
+      <c r="D1" s="2" t="inlineStr">
+        <is>
+          <t>Change</t>
+        </is>
+      </c>
+      <c r="E1" s="2" t="inlineStr">
+        <is>
+          <t>% Change</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" s="2" t="inlineStr">
+        <is>
+          <t>AXISBANK.NS</t>
+        </is>
+      </c>
+      <c r="B2" t="n">
+        <v>406.65</v>
+      </c>
+      <c r="C2" t="n">
+        <v>431.65</v>
+      </c>
+      <c r="D2" t="n">
+        <v>25</v>
+      </c>
+      <c r="E2" t="n">
+        <v>6.15</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" s="2" t="inlineStr">
+        <is>
+          <t>ASIANPAINT.NS</t>
+        </is>
+      </c>
+      <c r="B3" t="n">
+        <v>1683.39</v>
+      </c>
+      <c r="C3" t="n">
+        <v>1712.89</v>
+      </c>
+      <c r="D3" t="n">
+        <v>29.5</v>
+      </c>
+      <c r="E3" t="n">
+        <v>1.75</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" s="2" t="inlineStr">
+        <is>
+          <t>ADANIPORTS.NS</t>
+        </is>
+      </c>
+      <c r="B4" t="n">
+        <v>343.9</v>
+      </c>
+      <c r="C4" t="n">
+        <v>315.2</v>
+      </c>
+      <c r="D4" t="n">
+        <v>-28.7</v>
+      </c>
+      <c r="E4" t="n">
+        <v>-8.35</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet76.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:E4"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="2" t="inlineStr">
+        <is>
+          <t>MOMENTUM_ATH</t>
+        </is>
+      </c>
+      <c r="B1" s="2" t="inlineStr">
+        <is>
+          <t>2020-07-07</t>
+        </is>
+      </c>
+      <c r="C1" s="2" t="inlineStr">
+        <is>
+          <t>2020-08-07</t>
+        </is>
+      </c>
+      <c r="D1" s="2" t="inlineStr">
+        <is>
+          <t>Change</t>
+        </is>
+      </c>
+      <c r="E1" s="2" t="inlineStr">
+        <is>
+          <t>% Change</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" s="2" t="inlineStr">
+        <is>
+          <t>ASIANPAINT.NS</t>
+        </is>
+      </c>
+      <c r="B2" t="n">
+        <v>1741.55</v>
+      </c>
+      <c r="C2" t="n">
+        <v>1803.5</v>
+      </c>
+      <c r="D2" t="n">
+        <v>61.95</v>
+      </c>
+      <c r="E2" t="n">
+        <v>3.56</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" s="2" t="inlineStr">
+        <is>
+          <t>AXISBANK.NS</t>
+        </is>
+      </c>
+      <c r="B3" t="n">
+        <v>447.35</v>
+      </c>
+      <c r="C3" t="n">
+        <v>433.3</v>
+      </c>
+      <c r="D3" t="n">
+        <v>-14.05</v>
+      </c>
+      <c r="E3" t="n">
+        <v>-3.14</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" s="2" t="inlineStr">
+        <is>
+          <t>ADANIPORTS.NS</t>
+        </is>
+      </c>
+      <c r="B4" t="n">
+        <v>345.95</v>
+      </c>
+      <c r="C4" t="n">
+        <v>326.65</v>
+      </c>
+      <c r="D4" t="n">
+        <v>-19.3</v>
+      </c>
+      <c r="E4" t="n">
+        <v>-5.58</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet77.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:E4"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="2" t="inlineStr">
+        <is>
+          <t>MOMENTUM_ATH</t>
+        </is>
+      </c>
+      <c r="B1" s="2" t="inlineStr">
+        <is>
+          <t>2020-07-14</t>
+        </is>
+      </c>
+      <c r="C1" s="2" t="inlineStr">
+        <is>
+          <t>2020-08-14</t>
+        </is>
+      </c>
+      <c r="D1" s="2" t="inlineStr">
+        <is>
+          <t>Change</t>
+        </is>
+      </c>
+      <c r="E1" s="2" t="inlineStr">
+        <is>
+          <t>% Change</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" s="2" t="inlineStr">
+        <is>
+          <t>ADANIPORTS.NS</t>
+        </is>
+      </c>
+      <c r="B2" t="n">
+        <v>320.4</v>
+      </c>
+      <c r="C2" t="n">
+        <v>348.1</v>
+      </c>
+      <c r="D2" t="n">
+        <v>27.7</v>
+      </c>
+      <c r="E2" t="n">
+        <v>8.65</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" s="2" t="inlineStr">
+        <is>
+          <t>ASIANPAINT.NS</t>
+        </is>
+      </c>
+      <c r="B3" t="n">
+        <v>1684.34</v>
+      </c>
+      <c r="C3" t="n">
+        <v>1799.8</v>
+      </c>
+      <c r="D3" t="n">
+        <v>115.47</v>
+      </c>
+      <c r="E3" t="n">
+        <v>6.86</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" s="2" t="inlineStr">
+        <is>
+          <t>AXISBANK.NS</t>
+        </is>
+      </c>
+      <c r="B4" t="n">
+        <v>417.7</v>
+      </c>
+      <c r="C4" t="n">
+        <v>435.85</v>
+      </c>
+      <c r="D4" t="n">
+        <v>18.15</v>
+      </c>
+      <c r="E4" t="n">
+        <v>4.35</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet78.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:E4"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="2" t="inlineStr">
+        <is>
+          <t>MOMENTUM_ATH</t>
+        </is>
+      </c>
+      <c r="B1" s="2" t="inlineStr">
+        <is>
+          <t>2020-07-21</t>
+        </is>
+      </c>
+      <c r="C1" s="2" t="inlineStr">
+        <is>
+          <t>2020-08-21</t>
+        </is>
+      </c>
+      <c r="D1" s="2" t="inlineStr">
+        <is>
+          <t>Change</t>
+        </is>
+      </c>
+      <c r="E1" s="2" t="inlineStr">
+        <is>
+          <t>% Change</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" s="2" t="inlineStr">
+        <is>
+          <t>ASIANPAINT.NS</t>
+        </is>
+      </c>
+      <c r="B2" t="n">
+        <v>1720.1</v>
+      </c>
+      <c r="C2" t="n">
+        <v>1955.02</v>
+      </c>
+      <c r="D2" t="n">
+        <v>234.92</v>
+      </c>
+      <c r="E2" t="n">
+        <v>13.66</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" s="2" t="inlineStr">
+        <is>
+          <t>ADANIPORTS.NS</t>
+        </is>
+      </c>
+      <c r="B3" t="n">
+        <v>314.7</v>
+      </c>
+      <c r="C3" t="n">
+        <v>354.35</v>
+      </c>
+      <c r="D3" t="n">
+        <v>39.65</v>
+      </c>
+      <c r="E3" t="n">
+        <v>12.6</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" s="2" t="inlineStr">
+        <is>
+          <t>AXISBANK.NS</t>
+        </is>
+      </c>
+      <c r="B4" t="n">
+        <v>446.2</v>
+      </c>
+      <c r="C4" t="n">
+        <v>440.45</v>
+      </c>
+      <c r="D4" t="n">
+        <v>-5.75</v>
+      </c>
+      <c r="E4" t="n">
+        <v>-1.29</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet79.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:E4"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="2" t="inlineStr">
+        <is>
+          <t>MOMENTUM_ATH</t>
+        </is>
+      </c>
+      <c r="B1" s="2" t="inlineStr">
+        <is>
+          <t>2020-07-28</t>
+        </is>
+      </c>
+      <c r="C1" s="2" t="inlineStr">
+        <is>
+          <t>2020-08-28</t>
+        </is>
+      </c>
+      <c r="D1" s="2" t="inlineStr">
+        <is>
+          <t>Change</t>
+        </is>
+      </c>
+      <c r="E1" s="2" t="inlineStr">
+        <is>
+          <t>% Change</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" s="2" t="inlineStr">
+        <is>
+          <t>AXISBANK.NS</t>
+        </is>
+      </c>
+      <c r="B2" t="n">
+        <v>437.05</v>
+      </c>
+      <c r="C2" t="n">
+        <v>509.2</v>
+      </c>
+      <c r="D2" t="n">
+        <v>72.15000000000001</v>
+      </c>
+      <c r="E2" t="n">
+        <v>16.51</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" s="2" t="inlineStr">
+        <is>
+          <t>ADANIPORTS.NS</t>
+        </is>
+      </c>
+      <c r="B3" t="n">
+        <v>318.6</v>
+      </c>
+      <c r="C3" t="n">
+        <v>360.05</v>
+      </c>
+      <c r="D3" t="n">
+        <v>41.45</v>
+      </c>
+      <c r="E3" t="n">
+        <v>13.01</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" s="2" t="inlineStr">
+        <is>
+          <t>ASIANPAINT.NS</t>
+        </is>
+      </c>
+      <c r="B4" t="n">
+        <v>1756.97</v>
+      </c>
+      <c r="C4" t="n">
+        <v>1955.12</v>
+      </c>
+      <c r="D4" t="n">
+        <v>198.15</v>
+      </c>
+      <c r="E4" t="n">
+        <v>11.28</v>
       </c>
     </row>
   </sheetData>
@@ -52087,6 +54550,315 @@
 </worksheet>
 </file>
 
+<file path=xl/worksheets/sheet80.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:E4"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="2" t="inlineStr">
+        <is>
+          <t>MOMENTUM_ATH</t>
+        </is>
+      </c>
+      <c r="B1" s="2" t="inlineStr">
+        <is>
+          <t>2020-08-04</t>
+        </is>
+      </c>
+      <c r="C1" s="2" t="inlineStr">
+        <is>
+          <t>2020-09-04</t>
+        </is>
+      </c>
+      <c r="D1" s="2" t="inlineStr">
+        <is>
+          <t>Change</t>
+        </is>
+      </c>
+      <c r="E1" s="2" t="inlineStr">
+        <is>
+          <t>% Change</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" s="2" t="inlineStr">
+        <is>
+          <t>ASIANPAINT.NS</t>
+        </is>
+      </c>
+      <c r="B2" t="n">
+        <v>1711.34</v>
+      </c>
+      <c r="C2" t="n">
+        <v>1953.37</v>
+      </c>
+      <c r="D2" t="n">
+        <v>242.03</v>
+      </c>
+      <c r="E2" t="n">
+        <v>14.14</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" s="2" t="inlineStr">
+        <is>
+          <t>ADANIPORTS.NS</t>
+        </is>
+      </c>
+      <c r="B3" t="n">
+        <v>314.95</v>
+      </c>
+      <c r="C3" t="n">
+        <v>353</v>
+      </c>
+      <c r="D3" t="n">
+        <v>38.05</v>
+      </c>
+      <c r="E3" t="n">
+        <v>12.08</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" s="2" t="inlineStr">
+        <is>
+          <t>AXISBANK.NS</t>
+        </is>
+      </c>
+      <c r="B4" t="n">
+        <v>429.15</v>
+      </c>
+      <c r="C4" t="n">
+        <v>455.2</v>
+      </c>
+      <c r="D4" t="n">
+        <v>26.05</v>
+      </c>
+      <c r="E4" t="n">
+        <v>6.07</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet81.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:E4"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="2" t="inlineStr">
+        <is>
+          <t>MOMENTUM_ATH</t>
+        </is>
+      </c>
+      <c r="B1" s="2" t="inlineStr">
+        <is>
+          <t>2020-08-11</t>
+        </is>
+      </c>
+      <c r="C1" s="2" t="inlineStr">
+        <is>
+          <t>2020-09-11</t>
+        </is>
+      </c>
+      <c r="D1" s="2" t="inlineStr">
+        <is>
+          <t>Change</t>
+        </is>
+      </c>
+      <c r="E1" s="2" t="inlineStr">
+        <is>
+          <t>% Change</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" s="2" t="inlineStr">
+        <is>
+          <t>ASIANPAINT.NS</t>
+        </is>
+      </c>
+      <c r="B2" t="n">
+        <v>1786.82</v>
+      </c>
+      <c r="C2" t="n">
+        <v>2032.85</v>
+      </c>
+      <c r="D2" t="n">
+        <v>246.02</v>
+      </c>
+      <c r="E2" t="n">
+        <v>13.77</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" s="2" t="inlineStr">
+        <is>
+          <t>ADANIPORTS.NS</t>
+        </is>
+      </c>
+      <c r="B3" t="n">
+        <v>335</v>
+      </c>
+      <c r="C3" t="n">
+        <v>342.5</v>
+      </c>
+      <c r="D3" t="n">
+        <v>7.5</v>
+      </c>
+      <c r="E3" t="n">
+        <v>2.24</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" s="2" t="inlineStr">
+        <is>
+          <t>AXISBANK.NS</t>
+        </is>
+      </c>
+      <c r="B4" t="n">
+        <v>448</v>
+      </c>
+      <c r="C4" t="n">
+        <v>447.2</v>
+      </c>
+      <c r="D4" t="n">
+        <v>-0.8</v>
+      </c>
+      <c r="E4" t="n">
+        <v>-0.18</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet82.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:E4"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="2" t="inlineStr">
+        <is>
+          <t>MOMENTUM_ATH</t>
+        </is>
+      </c>
+      <c r="B1" s="2" t="inlineStr">
+        <is>
+          <t>2020-08-18</t>
+        </is>
+      </c>
+      <c r="C1" s="2" t="inlineStr">
+        <is>
+          <t>2020-09-18</t>
+        </is>
+      </c>
+      <c r="D1" s="2" t="inlineStr">
+        <is>
+          <t>Change</t>
+        </is>
+      </c>
+      <c r="E1" s="2" t="inlineStr">
+        <is>
+          <t>% Change</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" s="2" t="inlineStr">
+        <is>
+          <t>ASIANPAINT.NS</t>
+        </is>
+      </c>
+      <c r="B2" t="n">
+        <v>1871.24</v>
+      </c>
+      <c r="C2" t="n">
+        <v>2025.31</v>
+      </c>
+      <c r="D2" t="n">
+        <v>154.06</v>
+      </c>
+      <c r="E2" t="n">
+        <v>8.23</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" s="2" t="inlineStr">
+        <is>
+          <t>ADANIPORTS.NS</t>
+        </is>
+      </c>
+      <c r="B3" t="n">
+        <v>357.45</v>
+      </c>
+      <c r="C3" t="n">
+        <v>357.85</v>
+      </c>
+      <c r="D3" t="n">
+        <v>0.4</v>
+      </c>
+      <c r="E3" t="n">
+        <v>0.11</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" s="2" t="inlineStr">
+        <is>
+          <t>AXISBANK.NS</t>
+        </is>
+      </c>
+      <c r="B4" t="n">
+        <v>445.8</v>
+      </c>
+      <c r="C4" t="n">
+        <v>443.35</v>
+      </c>
+      <c r="D4" t="n">
+        <v>-2.45</v>
+      </c>
+      <c r="E4" t="n">
+        <v>-0.55</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>

</xml_diff>